<commit_message>
add new prop to rpdInfo
</commit_message>
<xml_diff>
--- a/RPDService.Backend/Data/Data.xlsx
+++ b/RPDService.Backend/Data/Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Projects\RPDService\Stash\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Projects\RPDService\RPDService.Backend\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74A09573-DD6E-4229-A568-32F3FBD3B646}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5866344D-24F7-4F85-8360-F3D3FFEDF092}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8850" yWindow="1665" windowWidth="28710" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2220" yWindow="5670" windowWidth="28710" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1067" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1068" uniqueCount="230">
   <si>
     <t>Факультет</t>
   </si>
@@ -712,6 +712,9 @@
   </si>
   <si>
     <t>Номер каф чит</t>
+  </si>
+  <si>
+    <t>Зачетные единицы</t>
   </si>
 </sst>
 </file>
@@ -742,7 +745,7 @@
       <charset val="204"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -753,6 +756,18 @@
       <patternFill patternType="solid">
         <fgColor indexed="22"/>
         <bgColor indexed="0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -784,7 +799,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -795,6 +810,13 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -1076,18 +1098,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S132"/>
+  <dimension ref="A1:T132"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U5" sqref="U5"/>
+    <sheetView tabSelected="1" topLeftCell="A124" workbookViewId="0">
+      <selection activeCell="V6" sqref="V6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="6" max="6" width="19.140625" customWidth="1"/>
+    <col min="20" max="20" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" ht="60" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1145,8 +1168,11 @@
       <c r="S1" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T1" s="4" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>14</v>
       </c>
@@ -1204,8 +1230,11 @@
       <c r="S2" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T2" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
@@ -1263,8 +1292,11 @@
       <c r="S3" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T3" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
@@ -1322,8 +1354,11 @@
       <c r="S4" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T4" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>25</v>
       </c>
@@ -1381,8 +1416,11 @@
       <c r="S5" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T5" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>25</v>
       </c>
@@ -1440,8 +1478,11 @@
       <c r="S6" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T6" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>25</v>
       </c>
@@ -1499,8 +1540,11 @@
       <c r="S7" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T7" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>31</v>
       </c>
@@ -1558,8 +1602,11 @@
       <c r="S8" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T8" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>31</v>
       </c>
@@ -1617,8 +1664,11 @@
       <c r="S9" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T9" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>36</v>
       </c>
@@ -1676,8 +1726,11 @@
       <c r="S10" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T10" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>14</v>
       </c>
@@ -1735,8 +1788,11 @@
       <c r="S11" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T11" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>14</v>
       </c>
@@ -1794,8 +1850,11 @@
       <c r="S12" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T12" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>14</v>
       </c>
@@ -1853,8 +1912,11 @@
       <c r="S13" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T13" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>31</v>
       </c>
@@ -1912,8 +1974,11 @@
       <c r="S14" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T14" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>46</v>
       </c>
@@ -1971,8 +2036,11 @@
       <c r="S15" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T15" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>25</v>
       </c>
@@ -2030,8 +2098,11 @@
       <c r="S16" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T16" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>25</v>
       </c>
@@ -2089,8 +2160,11 @@
       <c r="S17" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T17" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>25</v>
       </c>
@@ -2148,8 +2222,11 @@
       <c r="S18" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T18" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>25</v>
       </c>
@@ -2207,8 +2284,11 @@
       <c r="S19" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T19" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>25</v>
       </c>
@@ -2266,8 +2346,11 @@
       <c r="S20" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T20" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>31</v>
       </c>
@@ -2325,8 +2408,11 @@
       <c r="S21" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T21" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>31</v>
       </c>
@@ -2384,8 +2470,11 @@
       <c r="S22" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T22" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>60</v>
       </c>
@@ -2443,8 +2532,11 @@
       <c r="S23" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T23" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>60</v>
       </c>
@@ -2502,8 +2594,11 @@
       <c r="S24" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T24" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>25</v>
       </c>
@@ -2561,8 +2656,11 @@
       <c r="S25" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T25" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>25</v>
       </c>
@@ -2620,8 +2718,11 @@
       <c r="S26" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T26" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>25</v>
       </c>
@@ -2679,8 +2780,11 @@
       <c r="S27" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T27" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>25</v>
       </c>
@@ -2738,8 +2842,11 @@
       <c r="S28" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T28" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>25</v>
       </c>
@@ -2797,8 +2904,11 @@
       <c r="S29" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T29" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>25</v>
       </c>
@@ -2856,8 +2966,11 @@
       <c r="S30" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T30" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>46</v>
       </c>
@@ -2915,8 +3028,11 @@
       <c r="S31" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T31" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>31</v>
       </c>
@@ -2974,8 +3090,11 @@
       <c r="S32" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T32" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>31</v>
       </c>
@@ -3033,8 +3152,11 @@
       <c r="S33" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T33" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>60</v>
       </c>
@@ -3092,8 +3214,11 @@
       <c r="S34" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T34" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>14</v>
       </c>
@@ -3151,8 +3276,11 @@
       <c r="S35" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T35" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>14</v>
       </c>
@@ -3210,8 +3338,11 @@
       <c r="S36" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T36" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>14</v>
       </c>
@@ -3269,8 +3400,11 @@
       <c r="S37" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T37" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>31</v>
       </c>
@@ -3328,8 +3462,11 @@
       <c r="S38" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T38" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>31</v>
       </c>
@@ -3387,8 +3524,11 @@
       <c r="S39" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T39" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>14</v>
       </c>
@@ -3446,8 +3586,11 @@
       <c r="S40" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T40" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>14</v>
       </c>
@@ -3505,8 +3648,11 @@
       <c r="S41" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T41" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>87</v>
       </c>
@@ -3564,8 +3710,11 @@
       <c r="S42" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T42" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>87</v>
       </c>
@@ -3623,8 +3772,11 @@
       <c r="S43" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T43" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>31</v>
       </c>
@@ -3682,8 +3834,11 @@
       <c r="S44" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T44" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>31</v>
       </c>
@@ -3741,8 +3896,11 @@
       <c r="S45" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T45" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>31</v>
       </c>
@@ -3800,8 +3958,11 @@
       <c r="S46" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T46" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>25</v>
       </c>
@@ -3859,8 +4020,11 @@
       <c r="S47" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T47" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>25</v>
       </c>
@@ -3918,8 +4082,11 @@
       <c r="S48" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T48" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>25</v>
       </c>
@@ -3977,8 +4144,11 @@
       <c r="S49" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T49" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>31</v>
       </c>
@@ -4036,8 +4206,11 @@
       <c r="S50" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T50" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>31</v>
       </c>
@@ -4095,8 +4268,11 @@
       <c r="S51" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T51" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>39</v>
       </c>
@@ -4154,8 +4330,11 @@
       <c r="S52" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T52" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>31</v>
       </c>
@@ -4213,8 +4392,11 @@
       <c r="S53" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T53" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>39</v>
       </c>
@@ -4272,8 +4454,11 @@
       <c r="S54" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T54" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>39</v>
       </c>
@@ -4331,8 +4516,11 @@
       <c r="S55" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T55" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>106</v>
       </c>
@@ -4390,8 +4578,11 @@
       <c r="S56" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="57" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T56" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>31</v>
       </c>
@@ -4449,8 +4640,11 @@
       <c r="S57" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="58" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T57" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="58" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>39</v>
       </c>
@@ -4508,8 +4702,11 @@
       <c r="S58" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="59" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T58" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>39</v>
       </c>
@@ -4567,8 +4764,11 @@
       <c r="S59" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="60" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T59" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="60" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>39</v>
       </c>
@@ -4626,8 +4826,11 @@
       <c r="S60" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="61" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T60" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="61" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>39</v>
       </c>
@@ -4685,8 +4888,11 @@
       <c r="S61" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="62" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T61" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>39</v>
       </c>
@@ -4744,8 +4950,11 @@
       <c r="S62" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="63" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T62" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="63" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>39</v>
       </c>
@@ -4803,8 +5012,11 @@
       <c r="S63" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="64" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T63" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="64" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>39</v>
       </c>
@@ -4862,8 +5074,11 @@
       <c r="S64" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="65" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T64" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="65" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>39</v>
       </c>
@@ -4921,8 +5136,11 @@
       <c r="S65" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="66" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T65" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="66" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>39</v>
       </c>
@@ -4980,8 +5198,11 @@
       <c r="S66" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="67" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T66" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="67" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>39</v>
       </c>
@@ -5039,8 +5260,11 @@
       <c r="S67" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="68" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T67" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="68" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>39</v>
       </c>
@@ -5098,8 +5322,11 @@
       <c r="S68" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="69" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T68" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="69" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>60</v>
       </c>
@@ -5157,8 +5384,11 @@
       <c r="S69" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="70" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T69" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="70" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>39</v>
       </c>
@@ -5216,8 +5446,11 @@
       <c r="S70" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="71" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T70" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="71" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>39</v>
       </c>
@@ -5275,8 +5508,11 @@
       <c r="S71" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="72" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T71" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="72" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>60</v>
       </c>
@@ -5334,8 +5570,11 @@
       <c r="S72" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="73" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T72" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="73" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>87</v>
       </c>
@@ -5393,8 +5632,11 @@
       <c r="S73" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="74" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T73" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="74" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>87</v>
       </c>
@@ -5452,8 +5694,11 @@
       <c r="S74" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="75" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T74" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="75" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>87</v>
       </c>
@@ -5511,8 +5756,11 @@
       <c r="S75" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="76" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T75" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="76" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>87</v>
       </c>
@@ -5570,8 +5818,11 @@
       <c r="S76" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="77" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T76" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="77" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>31</v>
       </c>
@@ -5629,8 +5880,11 @@
       <c r="S77" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="78" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T77" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="78" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>14</v>
       </c>
@@ -5688,8 +5942,11 @@
       <c r="S78" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="79" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T78" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="79" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>14</v>
       </c>
@@ -5747,8 +6004,11 @@
       <c r="S79" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="80" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T79" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="80" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>14</v>
       </c>
@@ -5806,8 +6066,11 @@
       <c r="S80" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="81" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T80" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="81" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>87</v>
       </c>
@@ -5865,8 +6128,11 @@
       <c r="S81" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="82" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T81" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="82" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>14</v>
       </c>
@@ -5924,8 +6190,11 @@
       <c r="S82" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="83" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T82" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="83" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>14</v>
       </c>
@@ -5983,8 +6252,11 @@
       <c r="S83" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="84" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T83" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="84" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>60</v>
       </c>
@@ -6042,8 +6314,11 @@
       <c r="S84" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="85" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T84" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="85" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>60</v>
       </c>
@@ -6101,8 +6376,11 @@
       <c r="S85" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="86" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T85" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="86" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>60</v>
       </c>
@@ -6160,8 +6438,11 @@
       <c r="S86" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="87" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T86" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="87" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>36</v>
       </c>
@@ -6219,8 +6500,11 @@
       <c r="S87" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="88" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T87" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="88" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>60</v>
       </c>
@@ -6278,8 +6562,11 @@
       <c r="S88" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="89" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T88" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="89" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>14</v>
       </c>
@@ -6337,8 +6624,11 @@
       <c r="S89" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="90" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T89" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="90" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>39</v>
       </c>
@@ -6396,8 +6686,11 @@
       <c r="S90" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="91" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T90" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="91" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>39</v>
       </c>
@@ -6455,8 +6748,11 @@
       <c r="S91" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="92" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T91" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="92" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>46</v>
       </c>
@@ -6514,8 +6810,11 @@
       <c r="S92" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="93" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T92" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="93" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>31</v>
       </c>
@@ -6573,8 +6872,11 @@
       <c r="S93" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="94" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T93" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="94" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>46</v>
       </c>
@@ -6632,8 +6934,11 @@
       <c r="S94" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="95" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T94" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="95" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>31</v>
       </c>
@@ -6691,8 +6996,11 @@
       <c r="S95" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="96" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T95" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="96" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>31</v>
       </c>
@@ -6750,8 +7058,11 @@
       <c r="S96" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="97" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T96" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="97" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>14</v>
       </c>
@@ -6809,8 +7120,11 @@
       <c r="S97" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="98" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T97" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="98" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>46</v>
       </c>
@@ -6868,8 +7182,11 @@
       <c r="S98" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="99" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T98" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="99" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>46</v>
       </c>
@@ -6927,8 +7244,11 @@
       <c r="S99" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="100" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T99" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="100" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>60</v>
       </c>
@@ -6986,8 +7306,11 @@
       <c r="S100" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="101" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T100" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="101" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>60</v>
       </c>
@@ -7045,8 +7368,11 @@
       <c r="S101" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="102" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T101" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="102" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>39</v>
       </c>
@@ -7104,8 +7430,11 @@
       <c r="S102" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="103" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T102" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="103" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>87</v>
       </c>
@@ -7163,8 +7492,11 @@
       <c r="S103" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="104" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T103" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="104" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>31</v>
       </c>
@@ -7222,8 +7554,11 @@
       <c r="S104" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="105" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T104" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="105" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>31</v>
       </c>
@@ -7281,8 +7616,11 @@
       <c r="S105" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="106" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T105" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="106" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
         <v>106</v>
       </c>
@@ -7340,8 +7678,11 @@
       <c r="S106" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="107" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T106" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="107" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
         <v>106</v>
       </c>
@@ -7399,8 +7740,11 @@
       <c r="S107" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="108" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T107" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="108" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>187</v>
       </c>
@@ -7458,8 +7802,11 @@
       <c r="S108" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="109" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T108" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="109" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
         <v>14</v>
       </c>
@@ -7517,8 +7864,11 @@
       <c r="S109" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="110" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T109" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="110" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
         <v>60</v>
       </c>
@@ -7576,8 +7926,11 @@
       <c r="S110" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="111" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T110" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="111" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
         <v>60</v>
       </c>
@@ -7635,8 +7988,11 @@
       <c r="S111" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="112" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T111" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="112" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
         <v>87</v>
       </c>
@@ -7694,8 +8050,11 @@
       <c r="S112" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="113" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T112" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="113" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
         <v>87</v>
       </c>
@@ -7753,8 +8112,11 @@
       <c r="S113" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="114" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T113" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="114" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
         <v>87</v>
       </c>
@@ -7812,8 +8174,11 @@
       <c r="S114" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="115" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T114" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="115" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
         <v>87</v>
       </c>
@@ -7871,8 +8236,11 @@
       <c r="S115" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="116" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T115" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="116" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
         <v>87</v>
       </c>
@@ -7930,8 +8298,11 @@
       <c r="S116" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="117" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T116" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="117" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
         <v>87</v>
       </c>
@@ -7989,8 +8360,11 @@
       <c r="S117" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="118" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T117" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="118" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
         <v>60</v>
       </c>
@@ -8048,8 +8422,11 @@
       <c r="S118" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="119" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T118" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="119" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
         <v>60</v>
       </c>
@@ -8107,8 +8484,11 @@
       <c r="S119" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="120" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T119" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="120" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
         <v>87</v>
       </c>
@@ -8166,8 +8546,11 @@
       <c r="S120" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="121" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T120" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="121" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
         <v>60</v>
       </c>
@@ -8225,8 +8608,11 @@
       <c r="S121" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="122" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T121" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="122" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
         <v>60</v>
       </c>
@@ -8284,8 +8670,11 @@
       <c r="S122" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="123" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T122" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="123" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
         <v>60</v>
       </c>
@@ -8343,8 +8732,11 @@
       <c r="S123" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="124" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T123" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="124" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
         <v>60</v>
       </c>
@@ -8402,8 +8794,11 @@
       <c r="S124" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="125" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T124" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="125" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
         <v>60</v>
       </c>
@@ -8461,8 +8856,11 @@
       <c r="S125" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="126" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T125" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="126" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
         <v>60</v>
       </c>
@@ -8520,8 +8918,11 @@
       <c r="S126" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="127" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T126" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="127" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
         <v>60</v>
       </c>
@@ -8579,8 +8980,11 @@
       <c r="S127" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="128" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T127" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="128" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
         <v>60</v>
       </c>
@@ -8638,8 +9042,11 @@
       <c r="S128" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="129" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T128" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="129" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
         <v>60</v>
       </c>
@@ -8697,8 +9104,11 @@
       <c r="S129" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="130" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T129" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="130" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
         <v>60</v>
       </c>
@@ -8756,8 +9166,11 @@
       <c r="S130" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="131" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T130" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="131" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
         <v>36</v>
       </c>
@@ -8815,8 +9228,11 @@
       <c r="S131" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="132" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T131" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="132" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
         <v>46</v>
       </c>
@@ -8873,6 +9289,9 @@
       </c>
       <c r="S132" s="2" t="b">
         <v>1</v>
+      </c>
+      <c r="T132" s="5">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>